<commit_message>
add trap rain water
</commit_message>
<xml_diff>
--- a/problem_lists/高频100道题.xlsx
+++ b/problem_lists/高频100道题.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jingxi\Documents\WeChat Files\yu_jingxi\FileStorage\File\2020-05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jingxi\Documents\code\Leetcode_solutions\problem_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51640A1D-AAB0-444C-9E6B-693DB20B5500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2034CB9B-8C80-4A53-BF85-F54CAB78159F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15990" yWindow="2250" windowWidth="31230" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="33000" windowHeight="20235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="191">
   <si>
     <r>
       <rPr>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>https://www.lintcode.com/problem/text-justification/description</t>
+  </si>
+  <si>
+    <t>看了九章提示</t>
   </si>
 </sst>
 </file>
@@ -707,7 +710,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,6 +726,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39991454817346722"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,7 +768,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -790,6 +799,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,11 +823,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1089,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1102,16 +1123,17 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="40.28515625" customWidth="1"/>
     <col min="5" max="5" width="107.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.1" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="2"/>
@@ -1130,10 +1152,10 @@
     </row>
     <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="2"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1145,8 +1167,8 @@
     </row>
     <row r="4" spans="1:5" ht="18.75">
       <c r="A4" s="2"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1156,8 +1178,8 @@
     </row>
     <row r="5" spans="1:5" ht="18.75">
       <c r="A5" s="2"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1167,8 +1189,8 @@
     </row>
     <row r="6" spans="1:5" ht="18.75">
       <c r="A6" s="2"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
@@ -1178,8 +1200,8 @@
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="18.75">
       <c r="A7" s="2"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1189,8 +1211,8 @@
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="18.75">
       <c r="A8" s="2"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1200,8 +1222,8 @@
     </row>
     <row r="9" spans="1:5" ht="18.75">
       <c r="A9" s="2"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="8" t="s">
         <v>19</v>
       </c>
@@ -1211,8 +1233,8 @@
     </row>
     <row r="10" spans="1:5" ht="18.75">
       <c r="A10" s="2"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="8" t="s">
         <v>21</v>
       </c>
@@ -1222,8 +1244,8 @@
     </row>
     <row r="11" spans="1:5" ht="18.75">
       <c r="A11" s="2"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="8" t="s">
         <v>23</v>
       </c>
@@ -1233,8 +1255,8 @@
     </row>
     <row r="12" spans="1:5" ht="18.75">
       <c r="A12" s="2"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="8" t="s">
         <v>25</v>
       </c>
@@ -1244,8 +1266,8 @@
     </row>
     <row r="13" spans="1:5" ht="18.75">
       <c r="A13" s="2"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1257,8 +1279,8 @@
     </row>
     <row r="14" spans="1:5" ht="18.75">
       <c r="A14" s="2"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="8" t="s">
         <v>30</v>
       </c>
@@ -1268,8 +1290,8 @@
     </row>
     <row r="15" spans="1:5" ht="18.75">
       <c r="A15" s="2"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="6" t="s">
         <v>32</v>
       </c>
@@ -1279,8 +1301,8 @@
     </row>
     <row r="16" spans="1:5" ht="18.75">
       <c r="A16" s="2"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="8" t="s">
         <v>34</v>
       </c>
@@ -1288,10 +1310,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:7" ht="18" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="8" t="s">
         <v>36</v>
       </c>
@@ -1299,10 +1321,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1">
+    <row r="18" spans="1:7" ht="18" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="6" t="s">
         <v>38</v>
       </c>
@@ -1310,21 +1332,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1">
+    <row r="19" spans="1:7" ht="18" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="8" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1">
+      <c r="F19" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="18">
+        <v>44010</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="8" t="s">
         <v>42</v>
       </c>
@@ -1332,10 +1360,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1">
+    <row r="21" spans="1:7" ht="18" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="8" t="s">
         <v>44</v>
       </c>
@@ -1343,10 +1371,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1">
+    <row r="22" spans="1:7" ht="18" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="8" t="s">
         <v>46</v>
       </c>
@@ -1354,10 +1382,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1">
+    <row r="23" spans="1:7" ht="18" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -1367,10 +1395,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1">
+    <row r="24" spans="1:7" ht="18" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="8" t="s">
         <v>51</v>
       </c>
@@ -1378,10 +1406,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1">
+    <row r="25" spans="1:7" ht="18" customHeight="1">
       <c r="A25" s="2"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="6" t="s">
         <v>53</v>
       </c>
@@ -1389,10 +1417,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1">
+    <row r="26" spans="1:7" ht="18" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="6" t="s">
         <v>55</v>
       </c>
@@ -1400,10 +1428,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1">
+    <row r="27" spans="1:7" ht="18" customHeight="1">
       <c r="A27" s="2"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="6" t="s">
         <v>57</v>
       </c>
@@ -1411,12 +1439,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:7" ht="18" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -1426,9 +1454,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75">
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
+    <row r="29" spans="1:7" ht="18.75">
+      <c r="B29" s="17"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="4" t="s">
         <v>62</v>
       </c>
@@ -1436,9 +1464,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18.75">
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
+    <row r="30" spans="1:7" ht="18.75">
+      <c r="B30" s="17"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="6" t="s">
         <v>64</v>
       </c>
@@ -1446,9 +1474,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18.75">
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
+    <row r="31" spans="1:7" ht="18.75">
+      <c r="B31" s="17"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="6" t="s">
         <v>66</v>
       </c>
@@ -1456,9 +1484,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.75">
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
+    <row r="32" spans="1:7" ht="18.75">
+      <c r="B32" s="17"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="6" t="s">
         <v>68</v>
       </c>
@@ -1466,9 +1494,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="18.75">
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
+    <row r="33" spans="2:6" ht="18.75">
+      <c r="B33" s="17"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="6" t="s">
         <v>70</v>
       </c>
@@ -1476,9 +1504,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="18.75">
-      <c r="B34" s="12"/>
-      <c r="C34" s="14" t="s">
+    <row r="34" spans="2:6" ht="18.75">
+      <c r="B34" s="17"/>
+      <c r="C34" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -1488,9 +1516,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="18.75">
-      <c r="B35" s="12"/>
-      <c r="C35" s="14"/>
+    <row r="35" spans="2:6" ht="18.75">
+      <c r="B35" s="17"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="8" t="s">
         <v>74</v>
       </c>
@@ -1498,9 +1526,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="18.75">
-      <c r="B36" s="12"/>
-      <c r="C36" s="14"/>
+    <row r="36" spans="2:6" ht="18.75">
+      <c r="B36" s="17"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="6" t="s">
         <v>76</v>
       </c>
@@ -1508,9 +1536,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="18.75">
-      <c r="B37" s="12"/>
-      <c r="C37" s="14"/>
+    <row r="37" spans="2:6" ht="18.75">
+      <c r="B37" s="17"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="8" t="s">
         <v>78</v>
       </c>
@@ -1518,9 +1546,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="18.75">
-      <c r="B38" s="12"/>
-      <c r="C38" s="14"/>
+    <row r="38" spans="2:6" ht="18.75">
+      <c r="B38" s="17"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="8" t="s">
         <v>80</v>
       </c>
@@ -1528,9 +1556,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="18.75">
-      <c r="B39" s="12"/>
-      <c r="C39" s="14"/>
+    <row r="39" spans="2:6" ht="18.75">
+      <c r="B39" s="17"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="6" t="s">
         <v>82</v>
       </c>
@@ -1538,9 +1566,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="18.75">
-      <c r="B40" s="12"/>
-      <c r="C40" s="14"/>
+    <row r="40" spans="2:6" ht="18.75">
+      <c r="B40" s="17"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="8" t="s">
         <v>84</v>
       </c>
@@ -1548,9 +1576,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="18.75">
-      <c r="B41" s="12"/>
-      <c r="C41" s="14"/>
+    <row r="41" spans="2:6" ht="18.75">
+      <c r="B41" s="17"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="8" t="s">
         <v>86</v>
       </c>
@@ -1558,19 +1586,22 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="18.75">
-      <c r="B42" s="12"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="8" t="s">
+    <row r="42" spans="2:6" ht="18.75">
+      <c r="B42" s="17"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" ht="18.75">
-      <c r="B43" s="12"/>
-      <c r="C43" s="14"/>
+      <c r="F42" s="12">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="18.75">
+      <c r="B43" s="17"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="8" t="s">
         <v>90</v>
       </c>
@@ -1578,9 +1609,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="18.75">
-      <c r="B44" s="12"/>
-      <c r="C44" s="14"/>
+    <row r="44" spans="2:6" ht="18.75">
+      <c r="B44" s="17"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="8" t="s">
         <v>92</v>
       </c>
@@ -1588,9 +1619,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="18.75">
-      <c r="B45" s="12"/>
-      <c r="C45" s="14"/>
+    <row r="45" spans="2:6" ht="18.75">
+      <c r="B45" s="17"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="8" t="s">
         <v>94</v>
       </c>
@@ -1598,9 +1629,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="18.75">
-      <c r="B46" s="12"/>
-      <c r="C46" s="14"/>
+    <row r="46" spans="2:6" ht="18.75">
+      <c r="B46" s="17"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="6" t="s">
         <v>96</v>
       </c>
@@ -1608,9 +1639,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="18.75">
-      <c r="B47" s="12"/>
-      <c r="C47" s="14"/>
+    <row r="47" spans="2:6" ht="18.75">
+      <c r="B47" s="17"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="6" t="s">
         <v>98</v>
       </c>
@@ -1618,9 +1649,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="18.75">
-      <c r="B48" s="12"/>
-      <c r="C48" s="14"/>
+    <row r="48" spans="2:6" ht="18.75">
+      <c r="B48" s="17"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="6" t="s">
         <v>100</v>
       </c>
@@ -1629,8 +1660,8 @@
       </c>
     </row>
     <row r="49" spans="2:5" ht="18.75">
-      <c r="B49" s="12"/>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="17"/>
+      <c r="C49" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="8" t="s">
@@ -1641,8 +1672,8 @@
       </c>
     </row>
     <row r="50" spans="2:5" ht="18.75">
-      <c r="B50" s="12"/>
-      <c r="C50" s="13"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="8" t="s">
         <v>104</v>
       </c>
@@ -1651,8 +1682,8 @@
       </c>
     </row>
     <row r="51" spans="2:5" ht="18.75">
-      <c r="B51" s="12"/>
-      <c r="C51" s="13"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="6" t="s">
         <v>106</v>
       </c>
@@ -1661,8 +1692,8 @@
       </c>
     </row>
     <row r="52" spans="2:5" ht="18.75">
-      <c r="B52" s="12"/>
-      <c r="C52" s="13"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="6" t="s">
         <v>108</v>
       </c>
@@ -1671,10 +1702,10 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="18.75">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -1685,8 +1716,8 @@
       </c>
     </row>
     <row r="54" spans="2:5" ht="18.75">
-      <c r="B54" s="12"/>
-      <c r="C54" s="13"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="4" t="s">
         <v>9</v>
       </c>
@@ -1695,8 +1726,8 @@
       </c>
     </row>
     <row r="55" spans="2:5" ht="18.75">
-      <c r="B55" s="12"/>
-      <c r="C55" s="13"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="14"/>
       <c r="D55" s="6" t="s">
         <v>114</v>
       </c>
@@ -1705,8 +1736,8 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="18.75">
-      <c r="B56" s="12"/>
-      <c r="C56" s="13"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="14"/>
       <c r="D56" s="8" t="s">
         <v>116</v>
       </c>
@@ -1715,8 +1746,8 @@
       </c>
     </row>
     <row r="57" spans="2:5" ht="18.75">
-      <c r="B57" s="12"/>
-      <c r="C57" s="13"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="8" t="s">
         <v>118</v>
       </c>
@@ -1725,8 +1756,8 @@
       </c>
     </row>
     <row r="58" spans="2:5" ht="18.75">
-      <c r="B58" s="12"/>
-      <c r="C58" s="13"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="14"/>
       <c r="D58" s="6" t="s">
         <v>120</v>
       </c>
@@ -1735,8 +1766,8 @@
       </c>
     </row>
     <row r="59" spans="2:5" ht="18.75">
-      <c r="B59" s="12"/>
-      <c r="C59" s="13"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="8" t="s">
         <v>62</v>
       </c>
@@ -1745,8 +1776,8 @@
       </c>
     </row>
     <row r="60" spans="2:5" ht="18.75">
-      <c r="B60" s="12"/>
-      <c r="C60" s="13"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="14"/>
       <c r="D60" s="8" t="s">
         <v>17</v>
       </c>
@@ -1755,8 +1786,8 @@
       </c>
     </row>
     <row r="61" spans="2:5" ht="18.75">
-      <c r="B61" s="12"/>
-      <c r="C61" s="13"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="6" t="s">
         <v>19</v>
       </c>
@@ -1765,8 +1796,8 @@
       </c>
     </row>
     <row r="62" spans="2:5" ht="18.75">
-      <c r="B62" s="12"/>
-      <c r="C62" s="13"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="14"/>
       <c r="D62" s="6" t="s">
         <v>124</v>
       </c>
@@ -1775,8 +1806,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" ht="18.75">
-      <c r="B63" s="12"/>
-      <c r="C63" s="14" t="s">
+      <c r="B63" s="17"/>
+      <c r="C63" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D63" s="8" t="s">
@@ -1787,8 +1818,8 @@
       </c>
     </row>
     <row r="64" spans="2:5" ht="18.75">
-      <c r="B64" s="12"/>
-      <c r="C64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="13"/>
       <c r="D64" s="8" t="s">
         <v>128</v>
       </c>
@@ -1797,8 +1828,8 @@
       </c>
     </row>
     <row r="65" spans="2:5" ht="18.75">
-      <c r="B65" s="12"/>
-      <c r="C65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="13"/>
       <c r="D65" s="6" t="s">
         <v>130</v>
       </c>
@@ -1807,8 +1838,8 @@
       </c>
     </row>
     <row r="66" spans="2:5" ht="18.75">
-      <c r="B66" s="12"/>
-      <c r="C66" s="14"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="13"/>
       <c r="D66" s="8" t="s">
         <v>36</v>
       </c>
@@ -1817,8 +1848,8 @@
       </c>
     </row>
     <row r="67" spans="2:5" ht="18.75">
-      <c r="B67" s="12"/>
-      <c r="C67" s="14"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="13"/>
       <c r="D67" s="8" t="s">
         <v>133</v>
       </c>
@@ -1827,8 +1858,8 @@
       </c>
     </row>
     <row r="68" spans="2:5" ht="18.75">
-      <c r="B68" s="12"/>
-      <c r="C68" s="14"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="13"/>
       <c r="D68" s="6" t="s">
         <v>135</v>
       </c>
@@ -1837,8 +1868,8 @@
       </c>
     </row>
     <row r="69" spans="2:5" ht="18.75">
-      <c r="B69" s="12"/>
-      <c r="C69" s="14"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="13"/>
       <c r="D69" s="8" t="s">
         <v>137</v>
       </c>
@@ -1847,8 +1878,8 @@
       </c>
     </row>
     <row r="70" spans="2:5" ht="18.75">
-      <c r="B70" s="12"/>
-      <c r="C70" s="14"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="13"/>
       <c r="D70" s="8" t="s">
         <v>139</v>
       </c>
@@ -1857,8 +1888,8 @@
       </c>
     </row>
     <row r="71" spans="2:5" ht="18.75">
-      <c r="B71" s="12"/>
-      <c r="C71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="13"/>
       <c r="D71" s="8" t="s">
         <v>141</v>
       </c>
@@ -1867,8 +1898,8 @@
       </c>
     </row>
     <row r="72" spans="2:5" ht="18.75">
-      <c r="B72" s="12"/>
-      <c r="C72" s="14"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="13"/>
       <c r="D72" s="8" t="s">
         <v>143</v>
       </c>
@@ -1877,8 +1908,8 @@
       </c>
     </row>
     <row r="73" spans="2:5" ht="18.75">
-      <c r="B73" s="12"/>
-      <c r="C73" s="13" t="s">
+      <c r="B73" s="17"/>
+      <c r="C73" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D73" s="8" t="s">
@@ -1889,8 +1920,8 @@
       </c>
     </row>
     <row r="74" spans="2:5" ht="18.75">
-      <c r="B74" s="12"/>
-      <c r="C74" s="13"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="8" t="s">
         <v>53</v>
       </c>
@@ -1899,8 +1930,8 @@
       </c>
     </row>
     <row r="75" spans="2:5" ht="18.75">
-      <c r="B75" s="12"/>
-      <c r="C75" s="13"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="14"/>
       <c r="D75" s="6" t="s">
         <v>147</v>
       </c>
@@ -1909,8 +1940,8 @@
       </c>
     </row>
     <row r="76" spans="2:5" ht="18.75">
-      <c r="B76" s="12"/>
-      <c r="C76" s="13"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="14"/>
       <c r="D76" s="6" t="s">
         <v>149</v>
       </c>
@@ -1919,8 +1950,8 @@
       </c>
     </row>
     <row r="77" spans="2:5" ht="18.75">
-      <c r="B77" s="12"/>
-      <c r="C77" s="13"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="6" t="s">
         <v>151</v>
       </c>
@@ -1929,10 +1960,10 @@
       </c>
     </row>
     <row r="78" spans="2:5" ht="18.75">
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="6" t="s">
@@ -1943,8 +1974,8 @@
       </c>
     </row>
     <row r="79" spans="2:5" ht="18.75">
-      <c r="B79" s="12"/>
-      <c r="C79" s="13"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="14"/>
       <c r="D79" s="4" t="s">
         <v>9</v>
       </c>
@@ -1953,8 +1984,8 @@
       </c>
     </row>
     <row r="80" spans="2:5" ht="18.75">
-      <c r="B80" s="12"/>
-      <c r="C80" s="13"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="14"/>
       <c r="D80" s="6" t="s">
         <v>11</v>
       </c>
@@ -1963,8 +1994,8 @@
       </c>
     </row>
     <row r="81" spans="2:5" ht="18.75">
-      <c r="B81" s="12"/>
-      <c r="C81" s="13"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="8" t="s">
         <v>13</v>
       </c>
@@ -1973,8 +2004,8 @@
       </c>
     </row>
     <row r="82" spans="2:5" ht="18.75">
-      <c r="B82" s="12"/>
-      <c r="C82" s="13"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="8" t="s">
         <v>17</v>
       </c>
@@ -1983,8 +2014,8 @@
       </c>
     </row>
     <row r="83" spans="2:5" ht="18.75">
-      <c r="B83" s="12"/>
-      <c r="C83" s="14" t="s">
+      <c r="B83" s="17"/>
+      <c r="C83" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -1995,8 +2026,8 @@
       </c>
     </row>
     <row r="84" spans="2:5" ht="18.75">
-      <c r="B84" s="12"/>
-      <c r="C84" s="14"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="13"/>
       <c r="D84" s="8" t="s">
         <v>126</v>
       </c>
@@ -2005,8 +2036,8 @@
       </c>
     </row>
     <row r="85" spans="2:5" ht="18.75">
-      <c r="B85" s="12"/>
-      <c r="C85" s="14"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="13"/>
       <c r="D85" s="6" t="s">
         <v>130</v>
       </c>
@@ -2015,8 +2046,8 @@
       </c>
     </row>
     <row r="86" spans="2:5" ht="18.75">
-      <c r="B86" s="12"/>
-      <c r="C86" s="14"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="13"/>
       <c r="D86" s="8" t="s">
         <v>160</v>
       </c>
@@ -2025,8 +2056,8 @@
       </c>
     </row>
     <row r="87" spans="2:5" ht="18.75">
-      <c r="B87" s="12"/>
-      <c r="C87" s="14"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="13"/>
       <c r="D87" s="8" t="s">
         <v>162</v>
       </c>
@@ -2035,8 +2066,8 @@
       </c>
     </row>
     <row r="88" spans="2:5" ht="18.75">
-      <c r="B88" s="12"/>
-      <c r="C88" s="14"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="13"/>
       <c r="D88" s="6" t="s">
         <v>164</v>
       </c>
@@ -2045,8 +2076,8 @@
       </c>
     </row>
     <row r="89" spans="2:5" ht="18.75">
-      <c r="B89" s="12"/>
-      <c r="C89" s="14"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="13"/>
       <c r="D89" s="8" t="s">
         <v>137</v>
       </c>
@@ -2055,8 +2086,8 @@
       </c>
     </row>
     <row r="90" spans="2:5" ht="18.75">
-      <c r="B90" s="12"/>
-      <c r="C90" s="14"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="13"/>
       <c r="D90" s="8" t="s">
         <v>166</v>
       </c>
@@ -2065,8 +2096,8 @@
       </c>
     </row>
     <row r="91" spans="2:5" ht="18.75">
-      <c r="B91" s="12"/>
-      <c r="C91" s="14"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="13"/>
       <c r="D91" s="8" t="s">
         <v>168</v>
       </c>
@@ -2075,8 +2106,8 @@
       </c>
     </row>
     <row r="92" spans="2:5" ht="18.75">
-      <c r="B92" s="12"/>
-      <c r="C92" s="14"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="8" t="s">
         <v>170</v>
       </c>
@@ -2085,8 +2116,8 @@
       </c>
     </row>
     <row r="93" spans="2:5" ht="18.75">
-      <c r="B93" s="12"/>
-      <c r="C93" s="14"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="13"/>
       <c r="D93" s="6" t="s">
         <v>172</v>
       </c>
@@ -2095,8 +2126,8 @@
       </c>
     </row>
     <row r="94" spans="2:5" ht="18.75">
-      <c r="B94" s="12"/>
-      <c r="C94" s="14"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="13"/>
       <c r="D94" s="8" t="s">
         <v>174</v>
       </c>
@@ -2105,8 +2136,8 @@
       </c>
     </row>
     <row r="95" spans="2:5" ht="18.75">
-      <c r="B95" s="12"/>
-      <c r="C95" s="14"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="13"/>
       <c r="D95" s="8" t="s">
         <v>176</v>
       </c>
@@ -2115,8 +2146,8 @@
       </c>
     </row>
     <row r="96" spans="2:5" ht="18.75">
-      <c r="B96" s="12"/>
-      <c r="C96" s="14"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="8" t="s">
         <v>178</v>
       </c>
@@ -2125,8 +2156,8 @@
       </c>
     </row>
     <row r="97" spans="2:5" ht="18.75">
-      <c r="B97" s="12"/>
-      <c r="C97" s="14"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="13"/>
       <c r="D97" s="6" t="s">
         <v>180</v>
       </c>
@@ -2135,8 +2166,8 @@
       </c>
     </row>
     <row r="98" spans="2:5" ht="18.75">
-      <c r="B98" s="12"/>
-      <c r="C98" s="13" t="s">
+      <c r="B98" s="17"/>
+      <c r="C98" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D98" s="8" t="s">
@@ -2147,8 +2178,8 @@
       </c>
     </row>
     <row r="99" spans="2:5" ht="18.75">
-      <c r="B99" s="12"/>
-      <c r="C99" s="13"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="14"/>
       <c r="D99" s="8" t="s">
         <v>182</v>
       </c>
@@ -2157,8 +2188,8 @@
       </c>
     </row>
     <row r="100" spans="2:5" ht="18.75">
-      <c r="B100" s="12"/>
-      <c r="C100" s="13"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="14"/>
       <c r="D100" s="6" t="s">
         <v>184</v>
       </c>
@@ -2167,8 +2198,8 @@
       </c>
     </row>
     <row r="101" spans="2:5" ht="18.75">
-      <c r="B101" s="12"/>
-      <c r="C101" s="13"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="6" t="s">
         <v>186</v>
       </c>
@@ -2177,8 +2208,8 @@
       </c>
     </row>
     <row r="102" spans="2:5" ht="18.75">
-      <c r="B102" s="12"/>
-      <c r="C102" s="13"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="6" t="s">
         <v>188</v>
       </c>
@@ -2187,7 +2218,10 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="17">
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C97"/>
     <mergeCell ref="C98:C102"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B3:B27"/>
@@ -2203,8 +2237,6 @@
     <mergeCell ref="C53:C62"/>
     <mergeCell ref="C63:C72"/>
     <mergeCell ref="C73:C77"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C97"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>